<commit_message>
2020-07-21 JCS : ajout de A. Filatova
</commit_message>
<xml_diff>
--- a/GED-ALMA-PARAM-CodesStatistiquesSecondaires.xlsx
+++ b/GED-ALMA-PARAM-CodesStatistiquesSecondaires.xlsx
@@ -175,17 +175,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>PA</t>
+          <t>AF</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Pauline AUGE</t>
+          <t>Anna FILATOVA</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Pauline AUGE</t>
+          <t>Anna FILATOVA</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -195,11 +195,11 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>nicomo</t>
+          <t>jcs</t>
         </is>
       </c>
       <c r="G3" s="1" t="n">
-        <v>43858.0</v>
+        <v>44033.0</v>
       </c>
     </row>
     <row r="4">
@@ -210,17 +210,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>CBA</t>
+          <t>PA</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Céline BARBILLON</t>
+          <t>Pauline AUGE</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Céline BARBILLON</t>
+          <t>Pauline AUGE</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -230,11 +230,11 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>nicomo</t>
+          <t>jcs</t>
         </is>
       </c>
       <c r="G4" s="1" t="n">
-        <v>43858.0</v>
+        <v>44033.0</v>
       </c>
     </row>
     <row r="5">
@@ -245,17 +245,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>CBO</t>
+          <t>CBA</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Catherine BOUANICH</t>
+          <t>Céline BARBILLON</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Catherine BOUANICH</t>
+          <t>Céline BARBILLON</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -265,11 +265,11 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>nicomo</t>
+          <t>jcs</t>
         </is>
       </c>
       <c r="G5" s="1" t="n">
-        <v>43858.0</v>
+        <v>44033.0</v>
       </c>
     </row>
     <row r="6">
@@ -280,17 +280,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>SCA</t>
+          <t>CBO</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Sophia CAGNOLO</t>
+          <t>Catherine BOUANICH</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Sophia CAGNOLO</t>
+          <t>Catherine BOUANICH</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -300,11 +300,11 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>nicomo</t>
+          <t>jcs</t>
         </is>
       </c>
       <c r="G6" s="1" t="n">
-        <v>43858.0</v>
+        <v>44033.0</v>
       </c>
     </row>
     <row r="7">
@@ -315,17 +315,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>SCO</t>
+          <t>SCA</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Sandrine COLL</t>
+          <t>Sophia CAGNOLO</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Sandrine COLL</t>
+          <t>Sophia CAGNOLO</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -335,11 +335,11 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>nicomo</t>
+          <t>jcs</t>
         </is>
       </c>
       <c r="G7" s="1" t="n">
-        <v>43858.0</v>
+        <v>44033.0</v>
       </c>
     </row>
     <row r="8">
@@ -350,17 +350,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>CD</t>
+          <t>SCO</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Carine DESCHAMPS</t>
+          <t>Sandrine COLL</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Carine DESCHAMPS</t>
+          <t>Sandrine COLL</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -370,11 +370,11 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>nicomo</t>
+          <t>jcs</t>
         </is>
       </c>
       <c r="G8" s="1" t="n">
-        <v>43858.0</v>
+        <v>44033.0</v>
       </c>
     </row>
     <row r="9">
@@ -385,17 +385,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>DD</t>
+          <t>CD</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Dominique DIGUET</t>
+          <t>Carine DESCHAMPS</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Dominique DIGUET</t>
+          <t>Carine DESCHAMPS</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -405,11 +405,11 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>nicomo</t>
+          <t>jcs</t>
         </is>
       </c>
       <c r="G9" s="1" t="n">
-        <v>43858.0</v>
+        <v>44033.0</v>
       </c>
     </row>
     <row r="10">
@@ -420,17 +420,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>FF</t>
+          <t>DD</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Florence FERRI</t>
+          <t>Dominique DIGUET</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Florence FERRI</t>
+          <t>Dominique DIGUET</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -440,11 +440,11 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>nicomo</t>
+          <t>jcs</t>
         </is>
       </c>
       <c r="G10" s="1" t="n">
-        <v>43858.0</v>
+        <v>44033.0</v>
       </c>
     </row>
     <row r="11">
@@ -455,17 +455,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>RG</t>
+          <t>FF</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Rachel GUIDONI</t>
+          <t>Florence FERRI</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Rachel GUIDONI</t>
+          <t>Florence FERRI</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -475,11 +475,11 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>nicomo</t>
+          <t>jcs</t>
         </is>
       </c>
       <c r="G11" s="1" t="n">
-        <v>43858.0</v>
+        <v>44033.0</v>
       </c>
     </row>
     <row r="12">
@@ -490,17 +490,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>GH</t>
+          <t>RG</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Geoffrey HARAUX</t>
+          <t>Rachel GUIDONI</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Geoffrey HARAUX</t>
+          <t>Rachel GUIDONI</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -510,11 +510,11 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>nicomo</t>
+          <t>jcs</t>
         </is>
       </c>
       <c r="G12" s="1" t="n">
-        <v>43858.0</v>
+        <v>44033.0</v>
       </c>
     </row>
     <row r="13">
@@ -525,17 +525,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>BH</t>
+          <t>GH</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Brigitte HAUMONT</t>
+          <t>Geoffrey HARAUX</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Brigitte HAUMONT</t>
+          <t>Geoffrey HARAUX</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -545,11 +545,11 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>nicomo</t>
+          <t>jcs</t>
         </is>
       </c>
       <c r="G13" s="1" t="n">
-        <v>43858.0</v>
+        <v>44033.0</v>
       </c>
     </row>
     <row r="14">
@@ -560,17 +560,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>JL</t>
+          <t>BH</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Jeanne LONGEVIALLE</t>
+          <t>Brigitte HAUMONT</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Jeanne LONGEVIALLE</t>
+          <t>Brigitte HAUMONT</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -580,11 +580,11 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>nicomo</t>
+          <t>jcs</t>
         </is>
       </c>
       <c r="G14" s="1" t="n">
-        <v>43858.0</v>
+        <v>44033.0</v>
       </c>
     </row>
     <row r="15">
@@ -595,17 +595,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>FM</t>
+          <t>JL</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Fabrice MOUILLOT</t>
+          <t>Jeanne LONGEVIALLE</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Fabrice MOUILLOT</t>
+          <t>Jeanne LONGEVIALLE</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -615,11 +615,11 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>nicomo</t>
+          <t>jcs</t>
         </is>
       </c>
       <c r="G15" s="1" t="n">
-        <v>43858.0</v>
+        <v>44033.0</v>
       </c>
     </row>
     <row r="16">
@@ -630,17 +630,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>HP</t>
+          <t>FM</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Hélène POITEVIN</t>
+          <t>Fabrice MOUILLOT</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Hélène POITEVIN</t>
+          <t>Fabrice MOUILLOT</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -650,11 +650,11 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>nicomo</t>
+          <t>jcs</t>
         </is>
       </c>
       <c r="G16" s="1" t="n">
-        <v>43858.0</v>
+        <v>44033.0</v>
       </c>
     </row>
     <row r="17">
@@ -665,17 +665,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>HP</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Benjamin RINGARD</t>
+          <t>Hélène POITEVIN</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Benjamin RINGARD</t>
+          <t>Hélène POITEVIN</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -685,11 +685,11 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>nicomo</t>
+          <t>jcs</t>
         </is>
       </c>
       <c r="G17" s="1" t="n">
-        <v>43949.0</v>
+        <v>44033.0</v>
       </c>
     </row>
     <row r="18">
@@ -700,17 +700,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>FR</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Florence ROUILLER</t>
+          <t>Benjamin RINGARD</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Florence ROUILLER</t>
+          <t>Benjamin RINGARD</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -720,11 +720,11 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>nicomo</t>
+          <t>jcs</t>
         </is>
       </c>
       <c r="G18" s="1" t="n">
-        <v>43949.0</v>
+        <v>44033.0</v>
       </c>
     </row>
     <row r="19">
@@ -735,17 +735,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>DS</t>
+          <t>FR</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Daniela SCANCELLA</t>
+          <t>Florence ROUILLER</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Daniela SCANCELLA</t>
+          <t>Florence ROUILLER</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -755,11 +755,11 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>nicomo</t>
+          <t>jcs</t>
         </is>
       </c>
       <c r="G19" s="1" t="n">
-        <v>43949.0</v>
+        <v>44033.0</v>
       </c>
     </row>
     <row r="20">
@@ -770,31 +770,66 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
+          <t>DS</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Daniela SCANCELLA</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Daniela SCANCELLA</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>jcs</t>
+        </is>
+      </c>
+      <c r="G20" s="1" t="n">
+        <v>44033.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Oui</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
           <t>RT</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="C21" t="inlineStr">
         <is>
           <t>Robin TOUBLAN</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
+      <c r="D21" t="inlineStr">
         <is>
           <t>Robin TOUBLAN</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>nicomo</t>
-        </is>
-      </c>
-      <c r="G20" s="1" t="n">
-        <v>43949.0</v>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>jcs</t>
+        </is>
+      </c>
+      <c r="G21" s="1" t="n">
+        <v>44033.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>